<commit_message>
EPBDS-7063 Avoid static and read only fields in sugar constructor.
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-7063_NoDefaultConstructor/Main.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-7063_NoDefaultConstructor/Main.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\openl-tablets\STUDIO\org.openl.rules.test\test-resources\functionality\EPBDS-7063_NoDefaultConstructor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40B1651F-21C4-402B-B9FB-F11B3EA8C629}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06158241-BD90-4932-9AC6-565DA9FEC961}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12410" yWindow="2450" windowWidth="21550" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>Environment</t>
   </si>
@@ -35,6 +35,21 @@
   </si>
   <si>
     <t>return A1(field="hello");</t>
+  </si>
+  <si>
+    <t>org.openl.rules.beans.B1</t>
+  </si>
+  <si>
+    <t>Method B1 hello1()</t>
+  </si>
+  <si>
+    <t>return B1(name="hello");</t>
+  </si>
+  <si>
+    <t>Method B1 hello2()</t>
+  </si>
+  <si>
+    <t>return B1(var="hello");</t>
   </si>
 </sst>
 </file>
@@ -407,10 +422,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="B12:C18"/>
+  <dimension ref="B12:C27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -432,6 +447,14 @@
         <v>3</v>
       </c>
     </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" t="s">
+        <v>5</v>
+      </c>
+    </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>1</v>
@@ -440,6 +463,26 @@
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
EPBDS-13571 No error is displayed during the project compilation if the constructor accepts an invalid expression as input data
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-7063_NoDefaultConstructor/Main.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-7063_NoDefaultConstructor/Main.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\openl-tablets\STUDIO\org.openl.rules.test\test-resources\functionality\EPBDS-7063_NoDefaultConstructor\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mkama\.openl\user-workspace\admin\EPBDS-7063_NoDefaultConstructor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06158241-BD90-4932-9AC6-565DA9FEC961}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87E27076-DC1A-4866-B7B6-F0A7F83D9017}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12410" yWindow="2450" windowWidth="21550" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7840" yWindow="2690" windowWidth="27170" windowHeight="15040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Rules" sheetId="6" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>Environment</t>
   </si>
@@ -50,12 +50,37 @@
   </si>
   <si>
     <t>return B1(var="hello");</t>
+  </si>
+  <si>
+    <t>Datatype C1</t>
+  </si>
+  <si>
+    <t>String</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>Method C1 hello3()</t>
+  </si>
+  <si>
+    <t>return C1(name=wrongMethodCall("hello"));</t>
+  </si>
+  <si>
+    <t>Method String wrongMethodCall(int h)</t>
+  </si>
+  <si>
+    <t>return "hello"</t>
+  </si>
+  <si>
+    <t>return "hello";</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -80,10 +105,13 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -422,70 +450,107 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="B12:C27"/>
+  <dimension ref="B12:C42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="36.08984375" customWidth="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="13.81640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="36.08984375"/>
   </cols>
   <sheetData>
     <row r="12" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
+      <c r="B12" t="s" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
+      <c r="B13" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" t="s" s="0">
         <v>3</v>
       </c>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
+      <c r="B14" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" t="s" s="0">
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" t="s" s="0">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" t="s" s="0">
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21" t="s" s="0">
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B22" t="s" s="0">
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B26" t="s" s="0">
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B27" t="s" s="0">
         <v>9</v>
       </c>
     </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B31" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C31" s="1"/>
+    </row>
+    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B32" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="C32" t="s" s="0">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B36" t="s" s="0">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B37" t="s" s="0">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B41" t="s" s="0">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B42" t="s" s="0">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B31:C31"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>